<commit_message>
Remove ALU B mux and reroute switch to ACC.
</commit_message>
<xml_diff>
--- a/cpu_states.xlsx
+++ b/cpu_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wwcpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED832C-6C19-4BFE-A751-C7A22FD00834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE20554-C883-420F-A7B7-F8479FDD270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>S0</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>DATA --&gt; MDR</t>
-  </si>
-  <si>
-    <t>Reset ACC</t>
   </si>
   <si>
     <t>ACC + SW --&gt; DATA</t>
@@ -250,9 +247,6 @@
 Disable RAM output</t>
   </si>
   <si>
-    <t>DATA --&gt; IR</t>
-  </si>
-  <si>
     <t>0101 1010</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
   </si>
   <si>
     <t>MAR_SRC</t>
-  </si>
-  <si>
-    <t>ALU_SRC</t>
   </si>
   <si>
     <t>MAR_SRC = DATA</t>
@@ -285,6 +276,16 @@
   <si>
     <t>Enable RAM write
 MAR_SRC = PC</t>
+  </si>
+  <si>
+    <t>ACC_SRC</t>
+  </si>
+  <si>
+    <t>ACC_SRC = SW</t>
+  </si>
+  <si>
+    <t>DATA --&gt; IR
+ACC_SRC = DATA</t>
   </si>
 </sst>
 </file>
@@ -513,6 +514,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,9 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -852,25 +853,24 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -907,15 +907,15 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -930,9 +930,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -947,9 +947,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -964,9 +964,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -979,9 +979,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -996,9 +996,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -1009,9 +1009,9 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -1030,17 +1030,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1050,12 +1050,12 @@
         <v>18</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
@@ -1070,36 +1070,36 @@
         <v>30</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
@@ -1109,9 +1109,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1119,9 +1119,9 @@
       <c r="F14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
@@ -1143,33 +1143,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL37"/>
+  <dimension ref="A1:AL39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="37" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="37" ySplit="2" topLeftCell="AR6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA3" sqref="AA3"/>
+      <selection pane="bottomRight" activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="13" customWidth="1"/>
-    <col min="3" max="19" width="4.6640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="5.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="36" width="5.6640625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="5.6640625" style="13" customWidth="1"/>
-    <col min="38" max="38" width="9.109375" style="16"/>
+    <col min="1" max="1" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="13" customWidth="1"/>
+    <col min="3" max="19" width="4.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="5.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="36" width="5.7109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" style="13" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1180,7 +1180,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
@@ -1192,104 +1192,104 @@
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
       <c r="T1" s="22"/>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="25"/>
+    </row>
+    <row r="2" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="24"/>
-    </row>
-    <row r="2" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="29"/>
       <c r="T2" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AF2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AH2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AI2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AJ2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AK2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AK2" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="J3" s="1">
         <v>1</v>
@@ -1316,7 +1316,7 @@
       <c r="AJ3" s="13"/>
       <c r="AK3" s="17"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="I4" s="1">
         <v>1</v>
@@ -1341,7 +1341,7 @@
       <c r="AJ4" s="13"/>
       <c r="AK4" s="17"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="H5" s="1">
         <v>1</v>
@@ -1370,17 +1370,23 @@
       <c r="AJ5" s="13"/>
       <c r="AK5" s="17"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
         <v>1</v>
       </c>
       <c r="P6" s="1">
         <v>1</v>
       </c>
-      <c r="R6" s="1">
+      <c r="T6" s="1">
         <v>1</v>
       </c>
       <c r="U6" s="13"/>
@@ -1393,9 +1399,7 @@
       <c r="AB6" s="13"/>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13"/>
-      <c r="AE6" s="13">
-        <v>1</v>
-      </c>
+      <c r="AE6" s="13"/>
       <c r="AF6" s="13"/>
       <c r="AG6" s="13"/>
       <c r="AH6" s="13"/>
@@ -1403,9 +1407,9 @@
       <c r="AJ6" s="13"/>
       <c r="AK6" s="17"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -1414,9 +1418,6 @@
         <v>1</v>
       </c>
       <c r="R7" s="1">
-        <v>1</v>
-      </c>
-      <c r="S7" s="1">
         <v>1</v>
       </c>
       <c r="U7" s="13"/>
@@ -1439,9 +1440,9 @@
       <c r="AJ7" s="13"/>
       <c r="AK7" s="17"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1449,7 +1450,7 @@
       <c r="P8" s="1">
         <v>1</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>1</v>
       </c>
       <c r="S8" s="1">
@@ -1475,14 +1476,20 @@
       <c r="AJ8" s="13"/>
       <c r="AK8" s="17"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1">
         <v>1</v>
       </c>
       <c r="U9" s="13"/>
@@ -1495,35 +1502,27 @@
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13">
-        <v>1</v>
-      </c>
+      <c r="AE9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="13"/>
       <c r="AG9" s="13"/>
       <c r="AH9" s="13"/>
       <c r="AI9" s="13"/>
       <c r="AJ9" s="13"/>
       <c r="AK9" s="17"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="N10" s="1">
-        <v>1</v>
-      </c>
       <c r="O10" s="1">
         <v>1</v>
       </c>
-      <c r="P10" s="1">
-        <v>1</v>
-      </c>
-      <c r="U10" s="13">
-        <v>1</v>
-      </c>
+      <c r="U10" s="13"/>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
@@ -1534,24 +1533,37 @@
       <c r="AC10" s="13"/>
       <c r="AD10" s="13"/>
       <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
+      <c r="AF10" s="13">
+        <v>1</v>
+      </c>
       <c r="AG10" s="13"/>
       <c r="AH10" s="13"/>
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
       <c r="AK10" s="17"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="U11" s="13"/>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="13">
+        <v>1</v>
+      </c>
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
@@ -1563,30 +1575,23 @@
       <c r="AD11" s="13"/>
       <c r="AE11" s="13"/>
       <c r="AF11" s="13"/>
-      <c r="AG11" s="13">
-        <v>1</v>
-      </c>
+      <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
       <c r="AI11" s="13"/>
       <c r="AJ11" s="13"/>
       <c r="AK11" s="17"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1">
-        <v>1</v>
-      </c>
-      <c r="U12" s="13">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
@@ -1598,20 +1603,25 @@
       <c r="AD12" s="13"/>
       <c r="AE12" s="13"/>
       <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
+      <c r="AG12" s="13">
+        <v>1</v>
+      </c>
       <c r="AH12" s="13"/>
       <c r="AI12" s="13"/>
       <c r="AJ12" s="13"/>
       <c r="AK12" s="17"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="M13" s="1">
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
         <v>1</v>
       </c>
       <c r="U13" s="13">
@@ -1634,27 +1644,24 @@
       <c r="AJ13" s="13"/>
       <c r="AK13" s="17"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>1</v>
-      </c>
-      <c r="U14" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="U14" s="13">
+        <v>1</v>
+      </c>
       <c r="V14" s="13"/>
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
-      <c r="Z14" s="13">
-        <v>1</v>
-      </c>
+      <c r="Z14" s="13"/>
       <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
@@ -1667,27 +1674,27 @@
       <c r="AJ14" s="13"/>
       <c r="AK14" s="17"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="K15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
       </c>
       <c r="U15" s="13"/>
-      <c r="V15" s="13">
-        <v>1</v>
-      </c>
+      <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
+      <c r="Z15" s="13">
+        <v>1</v>
+      </c>
       <c r="AA15" s="13"/>
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
@@ -1700,20 +1707,17 @@
       <c r="AJ15" s="13"/>
       <c r="AK15" s="17"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
       <c r="N16" s="1">
-        <v>1</v>
-      </c>
-      <c r="O16" s="1">
-        <v>1</v>
-      </c>
-      <c r="P16" s="1">
         <v>1</v>
       </c>
       <c r="U16" s="13"/>
@@ -1736,14 +1740,23 @@
       <c r="AJ16" s="13"/>
       <c r="AK16" s="17"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1</v>
+      </c>
+      <c r="P17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17" s="1">
         <v>1</v>
       </c>
       <c r="U17" s="13"/>
@@ -1753,9 +1766,7 @@
       <c r="W17" s="13"/>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
-      <c r="Z17" s="13">
-        <v>1</v>
-      </c>
+      <c r="Z17" s="13"/>
       <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
@@ -1768,9 +1779,9 @@
       <c r="AJ17" s="13"/>
       <c r="AK17" s="17"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1778,42 +1789,39 @@
       <c r="M18" s="1">
         <v>1</v>
       </c>
-      <c r="O18" s="1">
-        <v>1</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1</v>
-      </c>
-      <c r="R18" s="1">
-        <v>1</v>
-      </c>
       <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
+      <c r="V18" s="13">
+        <v>1</v>
+      </c>
       <c r="W18" s="13"/>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
+      <c r="Z18" s="13">
+        <v>1</v>
+      </c>
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
-      <c r="AC18" s="13">
-        <v>1</v>
-      </c>
+      <c r="AC18" s="13"/>
       <c r="AD18" s="13"/>
       <c r="AE18" s="13"/>
       <c r="AF18" s="13"/>
       <c r="AG18" s="13"/>
-      <c r="AH18" s="13">
-        <v>1</v>
-      </c>
+      <c r="AH18" s="13"/>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="13"/>
       <c r="AK18" s="17"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1">
         <v>1</v>
       </c>
       <c r="P19" s="1">
@@ -1828,7 +1836,9 @@
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
       <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
+      <c r="AA19" s="13">
+        <v>1</v>
+      </c>
       <c r="AB19" s="13"/>
       <c r="AC19" s="13">
         <v>1</v>
@@ -1837,14 +1847,16 @@
       <c r="AE19" s="13"/>
       <c r="AF19" s="13"/>
       <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
+      <c r="AH19" s="13">
+        <v>1</v>
+      </c>
       <c r="AI19" s="13"/>
       <c r="AJ19" s="13"/>
       <c r="AK19" s="17"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1853,9 +1865,6 @@
         <v>1</v>
       </c>
       <c r="R20" s="1">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1">
         <v>1</v>
       </c>
       <c r="U20" s="13"/>
@@ -1869,9 +1878,7 @@
       <c r="AC20" s="13">
         <v>1</v>
       </c>
-      <c r="AD20" s="13">
-        <v>1</v>
-      </c>
+      <c r="AD20" s="13"/>
       <c r="AE20" s="13"/>
       <c r="AF20" s="13"/>
       <c r="AG20" s="13"/>
@@ -1880,9 +1887,9 @@
       <c r="AJ20" s="13"/>
       <c r="AK20" s="17"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1890,7 +1897,7 @@
       <c r="P21" s="1">
         <v>1</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>1</v>
       </c>
       <c r="S21" s="1">
@@ -1903,10 +1910,10 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
-      <c r="AB21" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13">
+        <v>1</v>
+      </c>
       <c r="AD21" s="13">
         <v>1</v>
       </c>
@@ -1918,9 +1925,9 @@
       <c r="AJ21" s="13"/>
       <c r="AK21" s="17"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1929,6 +1936,9 @@
         <v>1</v>
       </c>
       <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
         <v>1</v>
       </c>
       <c r="U22" s="13"/>
@@ -1942,7 +1952,9 @@
         <v>1</v>
       </c>
       <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
+      <c r="AD22" s="13">
+        <v>1</v>
+      </c>
       <c r="AE22" s="13"/>
       <c r="AF22" s="13"/>
       <c r="AG22" s="13"/>
@@ -1951,23 +1963,17 @@
       <c r="AJ22" s="13"/>
       <c r="AK22" s="17"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="M23" s="1">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1">
-        <v>1</v>
-      </c>
       <c r="P23" s="1">
         <v>1</v>
       </c>
-      <c r="R23" s="1">
+      <c r="Q23" s="1">
         <v>1</v>
       </c>
       <c r="U23" s="13"/>
@@ -1977,10 +1983,10 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="13">
-        <v>1</v>
-      </c>
+      <c r="AB23" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="13"/>
       <c r="AD23" s="13"/>
       <c r="AE23" s="13"/>
       <c r="AF23" s="13"/>
@@ -1990,11 +1996,17 @@
       <c r="AJ23" s="13"/>
       <c r="AK23" s="17"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="1">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
         <v>1</v>
       </c>
       <c r="P24" s="1">
@@ -2009,34 +2021,33 @@
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
+      <c r="AA24" s="13">
+        <v>1</v>
+      </c>
       <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
+      <c r="AC24" s="13">
+        <v>1</v>
+      </c>
       <c r="AD24" s="13"/>
       <c r="AE24" s="13"/>
       <c r="AF24" s="13"/>
       <c r="AG24" s="13"/>
       <c r="AH24" s="13"/>
-      <c r="AI24" s="13">
-        <v>1</v>
-      </c>
+      <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
       <c r="AK24" s="17"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="P25" s="1">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1">
-        <v>1</v>
-      </c>
-      <c r="S25" s="1">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25" s="1">
         <v>1</v>
       </c>
       <c r="U25" s="13"/>
@@ -2053,15 +2064,13 @@
       <c r="AF25" s="13"/>
       <c r="AG25" s="13"/>
       <c r="AH25" s="13"/>
-      <c r="AI25" s="13">
-        <v>1</v>
-      </c>
+      <c r="AI25" s="13"/>
       <c r="AJ25" s="13"/>
       <c r="AK25" s="17"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -2069,10 +2078,7 @@
       <c r="P26" s="1">
         <v>1</v>
       </c>
-      <c r="Q26" s="1">
-        <v>1</v>
-      </c>
-      <c r="S26" s="1">
+      <c r="R26" s="1">
         <v>1</v>
       </c>
       <c r="U26" s="13"/>
@@ -2095,9 +2101,9 @@
       <c r="AJ26" s="13"/>
       <c r="AK26" s="17"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -2105,7 +2111,10 @@
       <c r="P27" s="1">
         <v>1</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
+        <v>1</v>
+      </c>
+      <c r="S27" s="1">
         <v>1</v>
       </c>
       <c r="U27" s="13"/>
@@ -2128,17 +2137,20 @@
       <c r="AJ27" s="13"/>
       <c r="AK27" s="17"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="N28" s="1">
+      <c r="P28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="S28" s="1">
         <v>1</v>
       </c>
       <c r="U28" s="13"/>
@@ -2152,29 +2164,26 @@
       <c r="AC28" s="13"/>
       <c r="AD28" s="13"/>
       <c r="AE28" s="13"/>
-      <c r="AF28" s="13">
-        <v>1</v>
-      </c>
+      <c r="AF28" s="13"/>
       <c r="AG28" s="13"/>
       <c r="AH28" s="13"/>
-      <c r="AI28" s="13"/>
+      <c r="AI28" s="13">
+        <v>1</v>
+      </c>
       <c r="AJ28" s="13"/>
       <c r="AK28" s="17"/>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="N29" s="1">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1">
-        <v>1</v>
-      </c>
       <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
         <v>1</v>
       </c>
       <c r="U29" s="13"/>
@@ -2197,19 +2206,20 @@
       <c r="AJ29" s="13"/>
       <c r="AK29" s="17"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="M30" s="1">
-        <v>1</v>
-      </c>
-      <c r="U30" s="13">
-        <v>1</v>
-      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="U30" s="13"/>
       <c r="V30" s="13"/>
       <c r="W30" s="13"/>
       <c r="X30" s="13"/>
@@ -2220,21 +2230,23 @@
       <c r="AC30" s="13"/>
       <c r="AD30" s="13"/>
       <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
+      <c r="AF30" s="13">
+        <v>1</v>
+      </c>
       <c r="AG30" s="13"/>
       <c r="AH30" s="13"/>
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
       <c r="AK30" s="17"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>1</v>
       </c>
       <c r="O31" s="1">
@@ -2243,7 +2255,7 @@
       <c r="P31" s="1">
         <v>1</v>
       </c>
-      <c r="R31" s="1">
+      <c r="T31" s="1">
         <v>1</v>
       </c>
       <c r="U31" s="13"/>
@@ -2254,9 +2266,7 @@
       <c r="Z31" s="13"/>
       <c r="AA31" s="13"/>
       <c r="AB31" s="13"/>
-      <c r="AC31" s="13">
-        <v>1</v>
-      </c>
+      <c r="AC31" s="13"/>
       <c r="AD31" s="13"/>
       <c r="AE31" s="13"/>
       <c r="AF31" s="13"/>
@@ -2268,9 +2278,9 @@
       <c r="AJ31" s="13"/>
       <c r="AK31" s="17"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -2278,10 +2288,12 @@
       <c r="M32" s="1">
         <v>1</v>
       </c>
-      <c r="N32" s="1">
-        <v>1</v>
-      </c>
-      <c r="U32" s="13"/>
+      <c r="T32" s="1">
+        <v>1</v>
+      </c>
+      <c r="U32" s="13">
+        <v>1</v>
+      </c>
       <c r="V32" s="13"/>
       <c r="W32" s="13"/>
       <c r="X32" s="13"/>
@@ -2296,19 +2308,26 @@
       <c r="AG32" s="13"/>
       <c r="AH32" s="13"/>
       <c r="AI32" s="13"/>
-      <c r="AJ32" s="13">
-        <v>1</v>
-      </c>
+      <c r="AJ32" s="13"/>
       <c r="AK32" s="17"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="13">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="1">
         <v>1</v>
       </c>
       <c r="O33" s="1">
+        <v>1</v>
+      </c>
+      <c r="P33" s="1">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
         <v>1</v>
       </c>
       <c r="U33" s="13"/>
@@ -2317,28 +2336,32 @@
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
+      <c r="AA33" s="13">
+        <v>1</v>
+      </c>
       <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
+      <c r="AC33" s="13">
+        <v>1</v>
+      </c>
       <c r="AD33" s="13"/>
       <c r="AE33" s="13"/>
-      <c r="AF33" s="13">
-        <v>1</v>
-      </c>
+      <c r="AF33" s="13"/>
       <c r="AG33" s="13"/>
       <c r="AH33" s="13"/>
-      <c r="AI33" s="13"/>
+      <c r="AI33" s="13">
+        <v>1</v>
+      </c>
       <c r="AJ33" s="13"/>
       <c r="AK33" s="17"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="13">
-        <v>1</v>
-      </c>
-      <c r="K34" s="1">
+        <v>33</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="M34" s="1">
         <v>1</v>
       </c>
       <c r="N34" s="1">
@@ -2355,31 +2378,29 @@
       <c r="AC34" s="13"/>
       <c r="AD34" s="13"/>
       <c r="AE34" s="13"/>
-      <c r="AF34" s="13">
-        <v>1</v>
-      </c>
+      <c r="AF34" s="13"/>
       <c r="AG34" s="13"/>
       <c r="AH34" s="13"/>
       <c r="AI34" s="13"/>
-      <c r="AJ34" s="13"/>
+      <c r="AJ34" s="13">
+        <v>1</v>
+      </c>
       <c r="AK34" s="17"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B35" s="13">
         <v>1</v>
       </c>
-      <c r="M35" s="1">
+      <c r="O35" s="1">
         <v>1</v>
       </c>
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
       <c r="W35" s="13"/>
-      <c r="X35" s="13">
-        <v>1</v>
-      </c>
+      <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
       <c r="AA35" s="13"/>
@@ -2387,125 +2408,196 @@
       <c r="AC35" s="13"/>
       <c r="AD35" s="13"/>
       <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
+      <c r="AF35" s="13">
+        <v>1</v>
+      </c>
       <c r="AG35" s="13"/>
       <c r="AH35" s="13"/>
       <c r="AI35" s="13"/>
       <c r="AJ35" s="13"/>
       <c r="AK35" s="17"/>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1">
+        <v>1</v>
+      </c>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="13"/>
+      <c r="AF36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="13"/>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="17"/>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="13">
+        <v>1</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="13"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="13"/>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="17"/>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="13">
-        <v>1</v>
-      </c>
-      <c r="L36" s="1">
-        <v>1</v>
-      </c>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="18"/>
-      <c r="Z36" s="18"/>
-      <c r="AA36" s="18"/>
-      <c r="AB36" s="18"/>
-      <c r="AC36" s="18"/>
-      <c r="AD36" s="18"/>
-      <c r="AE36" s="18"/>
-      <c r="AF36" s="18"/>
-      <c r="AG36" s="18"/>
-      <c r="AH36" s="18"/>
-      <c r="AI36" s="18"/>
-      <c r="AJ36" s="18"/>
-      <c r="AK36" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="12">
-        <f>COUNT(U3:U36)</f>
+      <c r="B38" s="13">
+        <v>1</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="U38" s="18"/>
+      <c r="V38" s="18"/>
+      <c r="W38" s="18"/>
+      <c r="X38" s="18"/>
+      <c r="Y38" s="18"/>
+      <c r="Z38" s="18"/>
+      <c r="AA38" s="18"/>
+      <c r="AB38" s="18"/>
+      <c r="AC38" s="18"/>
+      <c r="AD38" s="18"/>
+      <c r="AE38" s="18"/>
+      <c r="AF38" s="18"/>
+      <c r="AG38" s="18"/>
+      <c r="AH38" s="18"/>
+      <c r="AI38" s="18"/>
+      <c r="AJ38" s="18"/>
+      <c r="AK38" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12">
+        <f>COUNT(T3:T38)</f>
+        <v>6</v>
+      </c>
+      <c r="U39" s="12">
+        <f>COUNT(U3:U38)</f>
         <v>5</v>
       </c>
-      <c r="V37" s="12">
-        <f t="shared" ref="V37:AK37" si="0">COUNT(V3:V36)</f>
+      <c r="V39" s="12">
+        <f t="shared" ref="V39:AK39" si="0">COUNT(V3:V38)</f>
         <v>4</v>
       </c>
-      <c r="W37" s="12">
+      <c r="W39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X37" s="12">
+      <c r="X39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Y37" s="12">
+      <c r="Y39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Z37" s="12">
+      <c r="Z39" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AA37" s="12"/>
-      <c r="AB37" s="12">
+      <c r="AA39" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AB39" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AC37" s="12">
+      <c r="AC39" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AD37" s="12">
+      <c r="AD39" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AE37" s="12">
+      <c r="AE39" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AF37" s="12">
+      <c r="AF39" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AG37" s="12">
+      <c r="AG39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AH37" s="12">
+      <c r="AH39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AI37" s="12">
+      <c r="AI39" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AJ37" s="12">
+      <c r="AJ39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AK37" s="12">
+      <c r="AK39" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Change out opcode to use ALU.
</commit_message>
<xml_diff>
--- a/cpu_states.xlsx
+++ b/cpu_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wwcpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C196E20-6873-4D17-84CC-7C687ECB483F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B991142-908C-4743-98F1-4C935A7EBC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>S0</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>0100 0000</t>
-  </si>
-  <si>
-    <t>0110 0000</t>
   </si>
   <si>
     <t>ZF</t>
@@ -335,6 +332,12 @@
   <si>
     <t>ACC_SRC = SW
 ACC = 0b001</t>
+  </si>
+  <si>
+    <t>ACC = 0b001</t>
+  </si>
+  <si>
+    <t>0110 1001</t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +585,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,21 +612,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -924,302 +951,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1623EA-A651-44FE-B5F6-3CCC41DCF92C}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="34" t="str">
+        <f>_xlfn.CONCAT("0x",BIN2HEX(SUBSTITUTE(A3," ",""),2))</f>
+        <v>0x0A</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="34" t="str">
+        <f t="shared" ref="B4:B15" si="0">_xlfn.CONCAT("0x",BIN2HEX(SUBSTITUTE(A4," ",""),2))</f>
+        <v>0x0B</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0D</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0C</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="H6" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="G6" s="3"/>
+      <c r="I6" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="1" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x20</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="I8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x20</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x38</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x40</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="I11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="I12" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="H12" s="33" t="s">
+      <c r="J12" s="23"/>
+      <c r="K12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x69</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="I13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>0x80</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="1" t="s">
+      <c r="G15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1267,7 +1353,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
@@ -1279,101 +1365,101 @@
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
       <c r="T1" s="22"/>
-      <c r="U1" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="26"/>
+      <c r="U1" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="29"/>
     </row>
     <row r="2" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="U2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA2" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AH2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AI2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AJ2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AK2" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AK2" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -1700,7 +1786,7 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1763,7 +1849,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1796,7 +1882,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2295,7 +2381,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -2506,7 +2592,7 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="13">
         <v>1</v>

</xml_diff>

<commit_message>
Fix RAM output enable.
</commit_message>
<xml_diff>
--- a/cpu_states.xlsx
+++ b/cpu_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wwcpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B991142-908C-4743-98F1-4C935A7EBC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766E04CF-4D85-47BA-A271-98BFB3C09A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49DCB9A7-1EE1-4A25-9D11-06E7B318AF4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -257,22 +257,10 @@
 ACC_SRC = DATA</t>
   </si>
   <si>
-    <t>ACC = 0b000</t>
-  </si>
-  <si>
-    <t>ACC = 0b011</t>
-  </si>
-  <si>
-    <t>ACC = 0b010</t>
-  </si>
-  <si>
-    <t>ACC = 0b101</t>
-  </si>
-  <si>
-    <t>ACC = 0b100</t>
-  </si>
-  <si>
     <t>0101 1001</t>
+  </si>
+  <si>
+    <t>0110 1001</t>
   </si>
   <si>
     <r>
@@ -287,7 +275,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ACC = 0b000</t>
+      <t>ALU = 0b000</t>
     </r>
   </si>
   <si>
@@ -302,7 +290,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ACC = 0b001</t>
+      <t>ALU = 0b001</t>
     </r>
     <r>
       <rPr>
@@ -317,27 +305,39 @@
     </r>
   </si>
   <si>
+    <t>ALU = 0b010</t>
+  </si>
+  <si>
+    <t>ALU = 0b000</t>
+  </si>
+  <si>
+    <t>ALU = 0b011</t>
+  </si>
+  <si>
+    <t>ALU = 0b101</t>
+  </si>
+  <si>
+    <t>ALU = 0b100</t>
+  </si>
+  <si>
     <t>Increment PC
-ACC = 0b000</t>
+ALU = 0b000</t>
   </si>
   <si>
     <t>Enable RAM output
-ACC = 0b000</t>
+ALU = 0b000</t>
   </si>
   <si>
     <t>Increment PC
 Enable RAM output
-ACC = 0b000</t>
+ALU = 0b000</t>
   </si>
   <si>
     <t>ACC_SRC = SW
-ACC = 0b001</t>
-  </si>
-  <si>
-    <t>ACC = 0b001</t>
-  </si>
-  <si>
-    <t>0110 1001</t>
+ALU = 0b001</t>
+  </si>
+  <si>
+    <t>ALU = 0b001</t>
   </si>
 </sst>
 </file>
@@ -594,6 +594,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,9 +613,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -620,17 +620,7 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -954,7 +944,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,13 +996,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I2" s="24"/>
     </row>
@@ -1020,7 +1010,7 @@
       <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="34" t="str">
+      <c r="B3" s="28" t="str">
         <f>_xlfn.CONCAT("0x",BIN2HEX(SUBSTITUTE(A3," ",""),2))</f>
         <v>0x0A</v>
       </c>
@@ -1031,7 +1021,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -1044,7 +1034,7 @@
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="34" t="str">
+      <c r="B4" s="28" t="str">
         <f t="shared" ref="B4:B15" si="0">_xlfn.CONCAT("0x",BIN2HEX(SUBSTITUTE(A4," ",""),2))</f>
         <v>0x0B</v>
       </c>
@@ -1055,7 +1045,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>17</v>
@@ -1068,7 +1058,7 @@
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="34" t="str">
+      <c r="B5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x0D</v>
       </c>
@@ -1079,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>18</v>
@@ -1092,7 +1082,7 @@
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="34" t="str">
+      <c r="B6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x0C</v>
       </c>
@@ -1101,7 +1091,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="I6" s="25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>19</v>
@@ -1114,7 +1104,7 @@
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="34" t="str">
+      <c r="B7" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x10</v>
       </c>
@@ -1126,7 +1116,7 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="25" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="1" t="s">
@@ -1137,7 +1127,7 @@
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="34" t="str">
+      <c r="B8" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x20</v>
       </c>
@@ -1146,7 +1136,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K8" s="3"/>
     </row>
@@ -1154,7 +1144,7 @@
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="34" t="str">
+      <c r="B9" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x20</v>
       </c>
@@ -1166,7 +1156,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>21</v>
@@ -1179,7 +1169,7 @@
       <c r="A10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="34" t="str">
+      <c r="B10" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x38</v>
       </c>
@@ -1193,7 +1183,7 @@
         <v>26</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>16</v>
@@ -1206,7 +1196,7 @@
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="34" t="str">
+      <c r="B11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x40</v>
       </c>
@@ -1220,7 +1210,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>67</v>
@@ -1234,9 +1224,9 @@
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="34" t="str">
+        <v>72</v>
+      </c>
+      <c r="B12" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x59</v>
       </c>
@@ -1245,7 +1235,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="I12" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J12" s="23"/>
       <c r="K12" s="1" t="s">
@@ -1254,9 +1244,9 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="34" t="str">
+        <v>73</v>
+      </c>
+      <c r="B13" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x69</v>
       </c>
@@ -1265,7 +1255,7 @@
       </c>
       <c r="G13" s="3"/>
       <c r="I13" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>32</v>
@@ -1275,7 +1265,7 @@
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="34" t="str">
+      <c r="B14" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
@@ -1289,7 +1279,7 @@
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="34" t="str">
+      <c r="B15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0x80</v>
       </c>
@@ -1304,7 +1294,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1365,52 +1355,52 @@
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
       <c r="T1" s="22"/>
-      <c r="U1" s="28" t="s">
+      <c r="U1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="30"/>
     </row>
     <row r="2" spans="1:37" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="34"/>
       <c r="T2" s="20" t="s">
         <v>66</v>
       </c>
@@ -1435,11 +1425,11 @@
       <c r="AA2" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="30" t="s">
+      <c r="AB2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
       <c r="AE2" s="8" t="s">
         <v>52</v>
       </c>

</xml_diff>